<commit_message>
works with by type  by age and uncond probs, weird issue with bytypes probs
</commit_message>
<xml_diff>
--- a/my_code/model_uncert/input/MH_trans.xlsx
+++ b/my_code/model_uncert/input/MH_trans.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="7">
   <si>
     <t>Bad MH Type : % transition from bad mental health</t>
   </si>
@@ -140,7 +140,7 @@
         <v>0.87653022511838263</v>
       </c>
       <c r="C3">
-        <v>0.12346977488161737</v>
+        <v>0.12346977488161738</v>
       </c>
       <c r="H3">
         <v>25</v>
@@ -164,7 +164,7 @@
         <v>25</v>
       </c>
       <c r="U3">
-        <v>0.78162556294991981</v>
+        <v>0.78162556294991992</v>
       </c>
       <c r="V3">
         <v>0.21837443705008014</v>
@@ -175,10 +175,10 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>0.87395627205409987</v>
+        <v>0.87395627205409998</v>
       </c>
       <c r="C4">
-        <v>0.1260437279459001</v>
+        <v>0.12604372794590013</v>
       </c>
       <c r="H4">
         <v>26</v>
@@ -193,7 +193,7 @@
         <v>26</v>
       </c>
       <c r="O4">
-        <v>0.29252559130432365</v>
+        <v>0.29252559130432371</v>
       </c>
       <c r="P4">
         <v>0.70747440869567635</v>
@@ -205,7 +205,7 @@
         <v>0.76819313097250685</v>
       </c>
       <c r="V4">
-        <v>0.23180686902749317</v>
+        <v>0.2318068690274932</v>
       </c>
     </row>
     <row r="5">
@@ -216,13 +216,13 @@
         <v>0.82499847165683271</v>
       </c>
       <c r="C5">
-        <v>0.17500152834316729</v>
+        <v>0.17500152834316726</v>
       </c>
       <c r="H5">
         <v>27</v>
       </c>
       <c r="I5">
-        <v>0.34404688368294079</v>
+        <v>0.34404688368294084</v>
       </c>
       <c r="J5">
         <v>0.65595311631705921</v>
@@ -231,10 +231,10 @@
         <v>27</v>
       </c>
       <c r="O5">
-        <v>0.25504018553691471</v>
+        <v>0.25504018553691477</v>
       </c>
       <c r="P5">
-        <v>0.74495981446308523</v>
+        <v>0.74495981446308535</v>
       </c>
       <c r="T5">
         <v>27</v>
@@ -243,7 +243,7 @@
         <v>0.77949984955494234</v>
       </c>
       <c r="V5">
-        <v>0.22050015044505775</v>
+        <v>0.22050015044505772</v>
       </c>
     </row>
     <row r="6">
@@ -251,37 +251,37 @@
         <v>28</v>
       </c>
       <c r="B6">
-        <v>0.8575775352415177</v>
+        <v>0.85757753524151781</v>
       </c>
       <c r="C6">
-        <v>0.14242246475848225</v>
+        <v>0.14242246475848228</v>
       </c>
       <c r="H6">
         <v>28</v>
       </c>
       <c r="I6">
-        <v>0.43625590660398045</v>
+        <v>0.43625590660398039</v>
       </c>
       <c r="J6">
-        <v>0.56374409339601961</v>
+        <v>0.5637440933960195</v>
       </c>
       <c r="N6">
         <v>28</v>
       </c>
       <c r="O6">
-        <v>0.18852078063785588</v>
+        <v>0.18852078063785591</v>
       </c>
       <c r="P6">
-        <v>0.81147921936214407</v>
+        <v>0.81147921936214418</v>
       </c>
       <c r="T6">
         <v>28</v>
       </c>
       <c r="U6">
-        <v>0.76977557193192436</v>
+        <v>0.76977557193192425</v>
       </c>
       <c r="V6">
-        <v>0.23022442806807569</v>
+        <v>0.23022442806807566</v>
       </c>
     </row>
     <row r="7">
@@ -292,7 +292,7 @@
         <v>0.84733845350568238</v>
       </c>
       <c r="C7">
-        <v>0.1526615464943176</v>
+        <v>0.15266154649431762</v>
       </c>
       <c r="H7">
         <v>29</v>
@@ -301,7 +301,7 @@
         <v>0.38002483683674088</v>
       </c>
       <c r="J7">
-        <v>0.61997516316325918</v>
+        <v>0.61997516316325907</v>
       </c>
       <c r="N7">
         <v>29</v>
@@ -330,13 +330,13 @@
         <v>0.8638401063512634</v>
       </c>
       <c r="C8">
-        <v>0.13615989364873654</v>
+        <v>0.13615989364873657</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8">
-        <v>0.40065277807806404</v>
+        <v>0.4006527780780641</v>
       </c>
       <c r="J8">
         <v>0.5993472219219359</v>
@@ -345,7 +345,7 @@
         <v>30</v>
       </c>
       <c r="O8">
-        <v>0.30478264439729863</v>
+        <v>0.30478264439729869</v>
       </c>
       <c r="P8">
         <v>0.69521735560270126</v>
@@ -354,7 +354,7 @@
         <v>30</v>
       </c>
       <c r="U8">
-        <v>0.77283425082552049</v>
+        <v>0.7728342508255206</v>
       </c>
       <c r="V8">
         <v>0.22716574917447951</v>
@@ -365,7 +365,7 @@
         <v>31</v>
       </c>
       <c r="B9">
-        <v>0.85775091610851661</v>
+        <v>0.85775091610851673</v>
       </c>
       <c r="C9">
         <v>0.14224908389148327</v>
@@ -383,7 +383,7 @@
         <v>31</v>
       </c>
       <c r="O9">
-        <v>0.17451785035030165</v>
+        <v>0.17451785035030168</v>
       </c>
       <c r="P9">
         <v>0.82548214964969835</v>
@@ -395,7 +395,7 @@
         <v>0.78478919227477728</v>
       </c>
       <c r="V9">
-        <v>0.21521080772522272</v>
+        <v>0.21521080772522275</v>
       </c>
     </row>
     <row r="10">
@@ -406,13 +406,13 @@
         <v>0.85664404815889494</v>
       </c>
       <c r="C10">
-        <v>0.14335595184110503</v>
+        <v>0.143355951841105</v>
       </c>
       <c r="H10">
         <v>32</v>
       </c>
       <c r="I10">
-        <v>0.47108405216680532</v>
+        <v>0.47108405216680543</v>
       </c>
       <c r="J10">
         <v>0.52891594783319462</v>
@@ -424,13 +424,13 @@
         <v>0.22054273529699958</v>
       </c>
       <c r="P10">
-        <v>0.77945726470300047</v>
+        <v>0.77945726470300036</v>
       </c>
       <c r="T10">
         <v>32</v>
       </c>
       <c r="U10">
-        <v>0.76208099822598852</v>
+        <v>0.7620809982259884</v>
       </c>
       <c r="V10">
         <v>0.23791900177401154</v>
@@ -444,7 +444,7 @@
         <v>0.84731293608230529</v>
       </c>
       <c r="C11">
-        <v>0.15268706391769471</v>
+        <v>0.15268706391769468</v>
       </c>
       <c r="H11">
         <v>33</v>
@@ -462,7 +462,7 @@
         <v>0.25181182832838944</v>
       </c>
       <c r="P11">
-        <v>0.74818817167161056</v>
+        <v>0.74818817167161045</v>
       </c>
       <c r="T11">
         <v>33</v>
@@ -471,7 +471,7 @@
         <v>0.78643712735741933</v>
       </c>
       <c r="V11">
-        <v>0.21356287264258073</v>
+        <v>0.2135628726425807</v>
       </c>
     </row>
     <row r="12">
@@ -482,16 +482,16 @@
         <v>0.85587686536535812</v>
       </c>
       <c r="C12">
-        <v>0.1441231346346418</v>
+        <v>0.14412313463464183</v>
       </c>
       <c r="H12">
         <v>34</v>
       </c>
       <c r="I12">
-        <v>0.43778042654786675</v>
+        <v>0.43778042654786681</v>
       </c>
       <c r="J12">
-        <v>0.56221957345213314</v>
+        <v>0.56221957345213325</v>
       </c>
       <c r="N12">
         <v>34</v>
@@ -526,7 +526,7 @@
         <v>35</v>
       </c>
       <c r="I13">
-        <v>0.42461608617338231</v>
+        <v>0.42461608617338237</v>
       </c>
       <c r="J13">
         <v>0.57538391382661769</v>
@@ -555,7 +555,7 @@
         <v>36</v>
       </c>
       <c r="B14">
-        <v>0.87660198513045695</v>
+        <v>0.87660198513045684</v>
       </c>
       <c r="C14">
         <v>0.12339801486954309</v>
@@ -573,7 +573,7 @@
         <v>36</v>
       </c>
       <c r="O14">
-        <v>0.29035277517603908</v>
+        <v>0.29035277517603914</v>
       </c>
       <c r="P14">
         <v>0.70964722482396081</v>
@@ -582,10 +582,10 @@
         <v>36</v>
       </c>
       <c r="U14">
-        <v>0.78837615300304353</v>
+        <v>0.78837615300304342</v>
       </c>
       <c r="V14">
-        <v>0.21162384699695655</v>
+        <v>0.21162384699695658</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>37</v>
       </c>
       <c r="B15">
-        <v>0.87026270089853586</v>
+        <v>0.87026270089853575</v>
       </c>
       <c r="C15">
-        <v>0.12973729910146425</v>
+        <v>0.12973729910146428</v>
       </c>
       <c r="H15">
         <v>37</v>
@@ -623,7 +623,7 @@
         <v>0.7858362350851662</v>
       </c>
       <c r="V15">
-        <v>0.21416376491483391</v>
+        <v>0.21416376491483394</v>
       </c>
     </row>
     <row r="16">
@@ -634,7 +634,7 @@
         <v>0.86479264499437936</v>
       </c>
       <c r="C16">
-        <v>0.1352073550056207</v>
+        <v>0.13520735500562067</v>
       </c>
       <c r="H16">
         <v>38</v>
@@ -643,7 +643,7 @@
         <v>0.40261529174044819</v>
       </c>
       <c r="J16">
-        <v>0.5973847082595517</v>
+        <v>0.59738470825955192</v>
       </c>
       <c r="N16">
         <v>38</v>
@@ -658,10 +658,10 @@
         <v>38</v>
       </c>
       <c r="U16">
-        <v>0.78457226335409846</v>
+        <v>0.78457226335409858</v>
       </c>
       <c r="V16">
-        <v>0.21542773664590145</v>
+        <v>0.21542773664590151</v>
       </c>
     </row>
     <row r="17">
@@ -678,7 +678,7 @@
         <v>39</v>
       </c>
       <c r="I17">
-        <v>0.41260760984041683</v>
+        <v>0.41260760984041694</v>
       </c>
       <c r="J17">
         <v>0.58739239015958311</v>
@@ -690,16 +690,16 @@
         <v>0.35062943925537354</v>
       </c>
       <c r="P17">
-        <v>0.6493705607446264</v>
+        <v>0.64937056074462651</v>
       </c>
       <c r="T17">
         <v>39</v>
       </c>
       <c r="U17">
-        <v>0.79352701221980604</v>
+        <v>0.79352701221980615</v>
       </c>
       <c r="V17">
-        <v>0.20647298778019391</v>
+        <v>0.20647298778019393</v>
       </c>
     </row>
     <row r="18">
@@ -707,7 +707,7 @@
         <v>40</v>
       </c>
       <c r="B18">
-        <v>0.87439011557987323</v>
+        <v>0.87439011557987312</v>
       </c>
       <c r="C18">
         <v>0.12560988442012688</v>
@@ -716,10 +716,10 @@
         <v>40</v>
       </c>
       <c r="I18">
-        <v>0.41596195468938324</v>
+        <v>0.41596195468938318</v>
       </c>
       <c r="J18">
-        <v>0.58403804531061687</v>
+        <v>0.58403804531061676</v>
       </c>
       <c r="N18">
         <v>40</v>
@@ -737,7 +737,7 @@
         <v>0.82303248300873932</v>
       </c>
       <c r="V18">
-        <v>0.17696751699126068</v>
+        <v>0.1769675169912607</v>
       </c>
     </row>
     <row r="19">
@@ -745,19 +745,19 @@
         <v>41</v>
       </c>
       <c r="B19">
-        <v>0.86043290398143446</v>
+        <v>0.85793586908031538</v>
       </c>
       <c r="C19">
-        <v>0.13956709601856554</v>
+        <v>0.14206413091968459</v>
       </c>
       <c r="H19">
         <v>41</v>
       </c>
       <c r="I19">
-        <v>0.42277551630385524</v>
+        <v>0.42514660142756766</v>
       </c>
       <c r="J19">
-        <v>0.57722448369614476</v>
+        <v>0.57485339857243234</v>
       </c>
       <c r="N19">
         <v>41</v>
@@ -766,13 +766,13 @@
         <v>0.23986285454067924</v>
       </c>
       <c r="P19">
-        <v>0.76013714545932087</v>
+        <v>0.76013714545932076</v>
       </c>
       <c r="T19">
         <v>41</v>
       </c>
       <c r="U19">
-        <v>0.82435037676105294</v>
+        <v>0.82435037676105305</v>
       </c>
       <c r="V19">
         <v>0.17564962323894703</v>
@@ -783,16 +783,16 @@
         <v>42</v>
       </c>
       <c r="B20">
-        <v>0.84948991742747637</v>
+        <v>0.84948991742747626</v>
       </c>
       <c r="C20">
-        <v>0.15051008257252368</v>
+        <v>0.15051008257252366</v>
       </c>
       <c r="H20">
         <v>42</v>
       </c>
       <c r="I20">
-        <v>0.38776856331023657</v>
+        <v>0.38776856331023662</v>
       </c>
       <c r="J20">
         <v>0.61223143668976343</v>
@@ -801,19 +801,19 @@
         <v>42</v>
       </c>
       <c r="O20">
-        <v>0.31229632190970419</v>
+        <v>0.30449261302319292</v>
       </c>
       <c r="P20">
-        <v>0.68770367809029576</v>
+        <v>0.69550738697680714</v>
       </c>
       <c r="T20">
         <v>42</v>
       </c>
       <c r="U20">
-        <v>0.80670108638972349</v>
+        <v>0.8089973912387497</v>
       </c>
       <c r="V20">
-        <v>0.19329891361027654</v>
+        <v>0.19100260876125033</v>
       </c>
     </row>
     <row r="21">
@@ -821,37 +821,37 @@
         <v>43</v>
       </c>
       <c r="B21">
-        <v>0.84706799450425552</v>
+        <v>0.84364005058323133</v>
       </c>
       <c r="C21">
-        <v>0.15293200549574451</v>
+        <v>0.1563599494167687</v>
       </c>
       <c r="H21">
         <v>43</v>
       </c>
       <c r="I21">
-        <v>0.36850038246576622</v>
+        <v>0.37118684893503323</v>
       </c>
       <c r="J21">
-        <v>0.63149961753423367</v>
+        <v>0.62881315106496671</v>
       </c>
       <c r="N21">
         <v>43</v>
       </c>
       <c r="O21">
-        <v>0.23884701823088497</v>
+        <v>0.23725529300605849</v>
       </c>
       <c r="P21">
-        <v>0.76115298176911506</v>
+        <v>0.76274470699394159</v>
       </c>
       <c r="T21">
         <v>43</v>
       </c>
       <c r="U21">
-        <v>0.81564232740318277</v>
+        <v>0.81624870645536263</v>
       </c>
       <c r="V21">
-        <v>0.18435767259681726</v>
+        <v>0.1837512935446374</v>
       </c>
     </row>
     <row r="22">
@@ -859,37 +859,37 @@
         <v>44</v>
       </c>
       <c r="B22">
-        <v>0.83593024208217692</v>
+        <v>0.8347830430598564</v>
       </c>
       <c r="C22">
-        <v>0.16406975791782313</v>
+        <v>0.16521695694014354</v>
       </c>
       <c r="H22">
         <v>44</v>
       </c>
       <c r="I22">
-        <v>0.4155020554318184</v>
+        <v>0.4165144892055892</v>
       </c>
       <c r="J22">
-        <v>0.58449794456818172</v>
+        <v>0.5834855107944108</v>
       </c>
       <c r="N22">
         <v>44</v>
       </c>
       <c r="O22">
-        <v>0.3350503611712109</v>
+        <v>0.3291341456689208</v>
       </c>
       <c r="P22">
-        <v>0.6649496388287891</v>
+        <v>0.67086585433107926</v>
       </c>
       <c r="T22">
         <v>44</v>
       </c>
       <c r="U22">
-        <v>0.81416166714340543</v>
+        <v>0.8157549975157472</v>
       </c>
       <c r="V22">
-        <v>0.18583833285659465</v>
+        <v>0.1842450024842528</v>
       </c>
     </row>
     <row r="23">
@@ -897,37 +897,37 @@
         <v>45</v>
       </c>
       <c r="B23">
-        <v>0.85070866375718712</v>
+        <v>0.85131864551493386</v>
       </c>
       <c r="C23">
-        <v>0.14929133624281288</v>
+        <v>0.1486813544850662</v>
       </c>
       <c r="H23">
         <v>45</v>
       </c>
       <c r="I23">
-        <v>0.44412031079816711</v>
+        <v>0.44045389805788204</v>
       </c>
       <c r="J23">
-        <v>0.55587968920183284</v>
+        <v>0.55954610194211796</v>
       </c>
       <c r="N23">
         <v>45</v>
       </c>
       <c r="O23">
-        <v>0.26099126309845583</v>
+        <v>0.25946755996903498</v>
       </c>
       <c r="P23">
-        <v>0.73900873690154412</v>
+        <v>0.74053244003096508</v>
       </c>
       <c r="T23">
         <v>45</v>
       </c>
       <c r="U23">
-        <v>0.81100361344969729</v>
+        <v>0.81154849605585644</v>
       </c>
       <c r="V23">
-        <v>0.18899638655030271</v>
+        <v>0.18845150394414351</v>
       </c>
     </row>
     <row r="24">
@@ -935,19 +935,19 @@
         <v>46</v>
       </c>
       <c r="B24">
-        <v>0.84886742994928488</v>
+        <v>0.84858951070180788</v>
       </c>
       <c r="C24">
-        <v>0.15113257005071518</v>
+        <v>0.15141048929819215</v>
       </c>
       <c r="H24">
         <v>46</v>
       </c>
       <c r="I24">
-        <v>0.45754754486056914</v>
+        <v>0.45349098558166445</v>
       </c>
       <c r="J24">
-        <v>0.54245245513943074</v>
+        <v>0.54650901441833555</v>
       </c>
       <c r="N24">
         <v>46</v>
@@ -962,10 +962,10 @@
         <v>46</v>
       </c>
       <c r="U24">
-        <v>0.80640921221095985</v>
+        <v>0.80640921221095996</v>
       </c>
       <c r="V24">
-        <v>0.19359078778904007</v>
+        <v>0.19359078778904013</v>
       </c>
     </row>
     <row r="25">
@@ -973,37 +973,37 @@
         <v>47</v>
       </c>
       <c r="B25">
-        <v>0.83944495126579977</v>
+        <v>0.83889778024881478</v>
       </c>
       <c r="C25">
-        <v>0.16055504873420021</v>
+        <v>0.16110221975118519</v>
       </c>
       <c r="H25">
         <v>47</v>
       </c>
       <c r="I25">
-        <v>0.33280742113103734</v>
+        <v>0.33313971320459579</v>
       </c>
       <c r="J25">
-        <v>0.66719257886896277</v>
+        <v>0.66686028679540421</v>
       </c>
       <c r="N25">
         <v>47</v>
       </c>
       <c r="O25">
-        <v>0.29173869110825401</v>
+        <v>0.29012002595273068</v>
       </c>
       <c r="P25">
-        <v>0.70826130889174599</v>
+        <v>0.70987997404726932</v>
       </c>
       <c r="T25">
         <v>47</v>
       </c>
       <c r="U25">
-        <v>0.8145122132383531</v>
+        <v>0.81502584979578829</v>
       </c>
       <c r="V25">
-        <v>0.18548778676164684</v>
+        <v>0.18497415020421179</v>
       </c>
     </row>
     <row r="26">
@@ -1011,25 +1011,25 @@
         <v>48</v>
       </c>
       <c r="B26">
-        <v>0.85297101004791309</v>
+        <v>0.85186122449884749</v>
       </c>
       <c r="C26">
-        <v>0.14702898995208688</v>
+        <v>0.14813877550115254</v>
       </c>
       <c r="H26">
         <v>48</v>
       </c>
       <c r="I26">
-        <v>0.37773759933749596</v>
+        <v>0.37853591146761412</v>
       </c>
       <c r="J26">
-        <v>0.62226240066250393</v>
+        <v>0.62146408853238577</v>
       </c>
       <c r="N26">
         <v>48</v>
       </c>
       <c r="O26">
-        <v>0.2378981645048952</v>
+        <v>0.23789816450489523</v>
       </c>
       <c r="P26">
         <v>0.7621018354951048</v>
@@ -1041,7 +1041,7 @@
         <v>0.81169744672528032</v>
       </c>
       <c r="V26">
-        <v>0.18830255327471965</v>
+        <v>0.18830255327471968</v>
       </c>
     </row>
     <row r="27">
@@ -1058,28 +1058,28 @@
         <v>49</v>
       </c>
       <c r="I27">
-        <v>0.35435746259444695</v>
+        <v>0.354357462594447</v>
       </c>
       <c r="J27">
-        <v>0.645642537405553</v>
+        <v>0.64564253740555311</v>
       </c>
       <c r="N27">
         <v>49</v>
       </c>
       <c r="O27">
-        <v>0.32149898989496783</v>
+        <v>0.31939909330795196</v>
       </c>
       <c r="P27">
-        <v>0.67850101010503205</v>
+        <v>0.68060090669204809</v>
       </c>
       <c r="T27">
         <v>49</v>
       </c>
       <c r="U27">
-        <v>0.81742900099179538</v>
+        <v>0.81792309769237825</v>
       </c>
       <c r="V27">
-        <v>0.18257099900820464</v>
+        <v>0.1820769023076218</v>
       </c>
     </row>
     <row r="28">
@@ -1087,25 +1087,25 @@
         <v>50</v>
       </c>
       <c r="B28">
-        <v>0.85166773682366104</v>
+        <v>0.85186685126229056</v>
       </c>
       <c r="C28">
-        <v>0.14833226317633888</v>
+        <v>0.14813314873770939</v>
       </c>
       <c r="H28">
         <v>50</v>
       </c>
       <c r="I28">
-        <v>0.41359984262553884</v>
+        <v>0.41226751499381536</v>
       </c>
       <c r="J28">
-        <v>0.58640015737446127</v>
+        <v>0.58773248500618469</v>
       </c>
       <c r="N28">
         <v>50</v>
       </c>
       <c r="O28">
-        <v>0.22249908709768457</v>
+        <v>0.22249908709768451</v>
       </c>
       <c r="P28">
         <v>0.77750091290231549</v>
@@ -1114,7 +1114,7 @@
         <v>50</v>
       </c>
       <c r="U28">
-        <v>0.81566785046289181</v>
+        <v>0.81566785046289192</v>
       </c>
       <c r="V28">
         <v>0.18433214953710816</v>
@@ -1125,19 +1125,19 @@
         <v>51</v>
       </c>
       <c r="B29">
-        <v>0.88024643766294264</v>
+        <v>0.87905042149343815</v>
       </c>
       <c r="C29">
-        <v>0.11975356233705745</v>
+        <v>0.12094957850656196</v>
       </c>
       <c r="H29">
         <v>51</v>
       </c>
       <c r="I29">
-        <v>0.39914091855054801</v>
+        <v>0.39995708216908094</v>
       </c>
       <c r="J29">
-        <v>0.60085908144945199</v>
+        <v>0.60004291783091912</v>
       </c>
       <c r="N29">
         <v>51</v>
@@ -1152,7 +1152,7 @@
         <v>51</v>
       </c>
       <c r="U29">
-        <v>0.83373935100438223</v>
+        <v>0.83373935100438235</v>
       </c>
       <c r="V29">
         <v>0.16626064899561771</v>
@@ -1166,34 +1166,34 @@
         <v>0.83472390137699326</v>
       </c>
       <c r="C30">
-        <v>0.16527609862300671</v>
+        <v>0.16527609862300668</v>
       </c>
       <c r="H30">
         <v>52</v>
       </c>
       <c r="I30">
-        <v>0.3915677642124219</v>
+        <v>0.39156776421242184</v>
       </c>
       <c r="J30">
-        <v>0.6084322357875781</v>
+        <v>0.60843223578757821</v>
       </c>
       <c r="N30">
         <v>52</v>
       </c>
       <c r="O30">
-        <v>0.27061031771008104</v>
+        <v>0.26740352399542389</v>
       </c>
       <c r="P30">
-        <v>0.72938968228991896</v>
+        <v>0.73259647600457622</v>
       </c>
       <c r="T30">
         <v>52</v>
       </c>
       <c r="U30">
-        <v>0.8233256449376718</v>
+        <v>0.82424421025453476</v>
       </c>
       <c r="V30">
-        <v>0.17667435506232815</v>
+        <v>0.17575578974546521</v>
       </c>
     </row>
     <row r="31">
@@ -1201,37 +1201,37 @@
         <v>53</v>
       </c>
       <c r="B31">
-        <v>0.87839797478307635</v>
+        <v>0.87853457289651848</v>
       </c>
       <c r="C31">
-        <v>0.12160202521692363</v>
+        <v>0.12146542710348164</v>
       </c>
       <c r="H31">
         <v>53</v>
       </c>
       <c r="I31">
-        <v>0.40362625438213789</v>
+        <v>0.40249498874583378</v>
       </c>
       <c r="J31">
-        <v>0.59637374561786216</v>
+        <v>0.59750501125416622</v>
       </c>
       <c r="N31">
         <v>53</v>
       </c>
       <c r="O31">
-        <v>0.27215100171922241</v>
+        <v>0.27062232157154659</v>
       </c>
       <c r="P31">
-        <v>0.72784899828077765</v>
+        <v>0.72937767842845347</v>
       </c>
       <c r="T31">
         <v>53</v>
       </c>
       <c r="U31">
-        <v>0.84659782549519835</v>
+        <v>0.84713189825869573</v>
       </c>
       <c r="V31">
-        <v>0.15340217450480167</v>
+        <v>0.15286810174130433</v>
       </c>
     </row>
     <row r="32">
@@ -1239,25 +1239,25 @@
         <v>54</v>
       </c>
       <c r="B32">
-        <v>0.87950821855950212</v>
+        <v>0.87963899154388892</v>
       </c>
       <c r="C32">
-        <v>0.12049178144049791</v>
+        <v>0.12036100845611108</v>
       </c>
       <c r="H32">
         <v>54</v>
       </c>
       <c r="I32">
-        <v>0.40670359745864654</v>
+        <v>0.40553059033009842</v>
       </c>
       <c r="J32">
-        <v>0.59329640254135352</v>
+        <v>0.59446940966990158</v>
       </c>
       <c r="N32">
         <v>54</v>
       </c>
       <c r="O32">
-        <v>0.2848790572551439</v>
+        <v>0.28487905725514384</v>
       </c>
       <c r="P32">
         <v>0.71512094274485616</v>
@@ -1269,7 +1269,7 @@
         <v>0.82439613788670441</v>
       </c>
       <c r="V32">
-        <v>0.17560386211329562</v>
+        <v>0.17560386211329565</v>
       </c>
     </row>
     <row r="33">
@@ -1277,19 +1277,19 @@
         <v>55</v>
       </c>
       <c r="B33">
-        <v>0.85739533018574088</v>
+        <v>0.85650654048257857</v>
       </c>
       <c r="C33">
-        <v>0.14260466981425901</v>
+        <v>0.14349345951742148</v>
       </c>
       <c r="H33">
         <v>55</v>
       </c>
       <c r="I33">
-        <v>0.39169695956001266</v>
+        <v>0.39243470091266691</v>
       </c>
       <c r="J33">
-        <v>0.60830304043998729</v>
+        <v>0.60756529908733314</v>
       </c>
       <c r="N33">
         <v>55</v>
@@ -1315,7 +1315,7 @@
         <v>56</v>
       </c>
       <c r="B34">
-        <v>0.87228754292915844</v>
+        <v>0.87228754292915833</v>
       </c>
       <c r="C34">
         <v>0.12771245707084158</v>
@@ -1324,7 +1324,7 @@
         <v>56</v>
       </c>
       <c r="I34">
-        <v>0.36601610997605316</v>
+        <v>0.36601610997605322</v>
       </c>
       <c r="J34">
         <v>0.63398389002394673</v>
@@ -1333,19 +1333,19 @@
         <v>56</v>
       </c>
       <c r="O34">
-        <v>0.32263686244651468</v>
+        <v>0.32095475894053055</v>
       </c>
       <c r="P34">
-        <v>0.67736313755348532</v>
+        <v>0.67904524105946928</v>
       </c>
       <c r="T34">
         <v>56</v>
       </c>
       <c r="U34">
-        <v>0.83641938750793388</v>
+        <v>0.83683209644202927</v>
       </c>
       <c r="V34">
-        <v>0.1635806124920661</v>
+        <v>0.16316790355797078</v>
       </c>
     </row>
     <row r="35">
@@ -1356,7 +1356,7 @@
         <v>0.86106173457017532</v>
       </c>
       <c r="C35">
-        <v>0.13893826542982471</v>
+        <v>0.13893826542982474</v>
       </c>
       <c r="H35">
         <v>57</v>
@@ -1365,7 +1365,7 @@
         <v>0.40828431423230471</v>
       </c>
       <c r="J35">
-        <v>0.59171568576769529</v>
+        <v>0.5917156857676954</v>
       </c>
       <c r="N35">
         <v>57</v>
@@ -1418,7 +1418,7 @@
         <v>58</v>
       </c>
       <c r="U36">
-        <v>0.84602591911032954</v>
+        <v>0.84602591911032943</v>
       </c>
       <c r="V36">
         <v>0.15397408088967052</v>
@@ -1429,37 +1429,37 @@
         <v>59</v>
       </c>
       <c r="B37">
-        <v>0.86003785623028572</v>
+        <v>0.86021979863514531</v>
       </c>
       <c r="C37">
-        <v>0.13996214376971425</v>
+        <v>0.13978020136485475</v>
       </c>
       <c r="H37">
         <v>59</v>
       </c>
       <c r="I37">
-        <v>0.4037748331612025</v>
+        <v>0.40259047389609087</v>
       </c>
       <c r="J37">
-        <v>0.59622516683879756</v>
+        <v>0.59740952610390918</v>
       </c>
       <c r="N37">
         <v>59</v>
       </c>
       <c r="O37">
-        <v>0.28954711466858724</v>
+        <v>0.28741565832641031</v>
       </c>
       <c r="P37">
-        <v>0.71045288533141282</v>
+        <v>0.71258434167358964</v>
       </c>
       <c r="T37">
         <v>59</v>
       </c>
       <c r="U37">
-        <v>0.83322713978533003</v>
+        <v>0.83363514062836896</v>
       </c>
       <c r="V37">
-        <v>0.16677286021467005</v>
+        <v>0.16636485937163115</v>
       </c>
     </row>
     <row r="38">
@@ -1467,37 +1467,37 @@
         <v>60</v>
       </c>
       <c r="B38">
-        <v>0.85322248454475302</v>
+        <v>0.85342624043529158</v>
       </c>
       <c r="C38">
-        <v>0.14677751545524703</v>
+        <v>0.14657375956470839</v>
       </c>
       <c r="H38">
         <v>60</v>
       </c>
       <c r="I38">
-        <v>0.40949481249937136</v>
+        <v>0.40834395649540894</v>
       </c>
       <c r="J38">
-        <v>0.59050518750062864</v>
+        <v>0.591656043504591</v>
       </c>
       <c r="N38">
         <v>60</v>
       </c>
       <c r="O38">
-        <v>0.3062447429428139</v>
+        <v>0.30624474294281384</v>
       </c>
       <c r="P38">
-        <v>0.69375525705718621</v>
+        <v>0.6937552570571861</v>
       </c>
       <c r="T38">
         <v>60</v>
       </c>
       <c r="U38">
-        <v>0.85583183635213922</v>
+        <v>0.85583183635213933</v>
       </c>
       <c r="V38">
-        <v>0.14416816364786075</v>
+        <v>0.14416816364786078</v>
       </c>
     </row>
     <row r="39">
@@ -1505,10 +1505,10 @@
         <v>61</v>
       </c>
       <c r="B39">
-        <v>0.84998765135052923</v>
+        <v>0.84998765135052912</v>
       </c>
       <c r="C39">
-        <v>0.1500123486494708</v>
+        <v>0.15001234864947077</v>
       </c>
       <c r="H39">
         <v>61</v>
@@ -1517,13 +1517,13 @@
         <v>0.38896417708499653</v>
       </c>
       <c r="J39">
-        <v>0.61103582291500336</v>
+        <v>0.61103582291500347</v>
       </c>
       <c r="N39">
         <v>61</v>
       </c>
       <c r="O39">
-        <v>0.30332949025461164</v>
+        <v>0.3033294902546117</v>
       </c>
       <c r="P39">
         <v>0.69667050974538836</v>
@@ -1552,10 +1552,10 @@
         <v>62</v>
       </c>
       <c r="I40">
-        <v>0.38308859914801358</v>
+        <v>0.38308859914801352</v>
       </c>
       <c r="J40">
-        <v>0.61691140085198648</v>
+        <v>0.61691140085198637</v>
       </c>
       <c r="N40">
         <v>62</v>
@@ -1570,10 +1570,10 @@
         <v>62</v>
       </c>
       <c r="U40">
-        <v>0.86691667206327561</v>
+        <v>0.86691667206327572</v>
       </c>
       <c r="V40">
-        <v>0.13308332793672428</v>
+        <v>0.13308332793672431</v>
       </c>
     </row>
     <row r="41">
@@ -1581,7 +1581,7 @@
         <v>63</v>
       </c>
       <c r="B41">
-        <v>0.88656404554817192</v>
+        <v>0.88656404554817181</v>
       </c>
       <c r="C41">
         <v>0.11343595445182811</v>
@@ -1593,16 +1593,16 @@
         <v>0.36656705881430607</v>
       </c>
       <c r="J41">
-        <v>0.63343294118569393</v>
+        <v>0.63343294118569382</v>
       </c>
       <c r="N41">
         <v>63</v>
       </c>
       <c r="O41">
-        <v>0.19932539841315877</v>
+        <v>0.1993253984131588</v>
       </c>
       <c r="P41">
-        <v>0.80067460158684112</v>
+        <v>0.80067460158684123</v>
       </c>
       <c r="T41">
         <v>63</v>
@@ -1611,7 +1611,7 @@
         <v>0.86706949290065805</v>
       </c>
       <c r="V41">
-        <v>0.13293050709934195</v>
+        <v>0.13293050709934198</v>
       </c>
     </row>
     <row r="42">
@@ -1622,13 +1622,13 @@
         <v>0.81927843129139422</v>
       </c>
       <c r="C42">
-        <v>0.18072156870860587</v>
+        <v>0.18072156870860584</v>
       </c>
       <c r="H42">
         <v>64</v>
       </c>
       <c r="I42">
-        <v>0.35214059788009816</v>
+        <v>0.35214059788009811</v>
       </c>
       <c r="J42">
         <v>0.64785940211990189</v>
@@ -1637,7 +1637,7 @@
         <v>64</v>
       </c>
       <c r="O42">
-        <v>0.35849468263281997</v>
+        <v>0.35849468263282003</v>
       </c>
       <c r="P42">
         <v>0.64150531736717997</v>
@@ -1660,13 +1660,13 @@
         <v>0.86843454229518435</v>
       </c>
       <c r="C43">
-        <v>0.13156545770481567</v>
+        <v>0.1315654577048157</v>
       </c>
       <c r="H43">
         <v>65</v>
       </c>
       <c r="I43">
-        <v>0.29884290842599182</v>
+        <v>0.29884290842599187</v>
       </c>
       <c r="J43">
         <v>0.70115709157400807</v>
@@ -1678,13 +1678,13 @@
         <v>0.30739433126140997</v>
       </c>
       <c r="P43">
-        <v>0.69260566873858997</v>
+        <v>0.69260566873859009</v>
       </c>
       <c r="T43">
         <v>65</v>
       </c>
       <c r="U43">
-        <v>0.875890643360143</v>
+        <v>0.87589064336014288</v>
       </c>
       <c r="V43">
         <v>0.12410935663985706</v>
@@ -1698,7 +1698,7 @@
         <v>0.86583262153772211</v>
       </c>
       <c r="C44">
-        <v>0.13416737846227789</v>
+        <v>0.13416737846227786</v>
       </c>
       <c r="H44">
         <v>66</v>
@@ -1716,16 +1716,16 @@
         <v>0.25119319271276486</v>
       </c>
       <c r="P44">
-        <v>0.74880680728723503</v>
+        <v>0.74880680728723514</v>
       </c>
       <c r="T44">
         <v>66</v>
       </c>
       <c r="U44">
-        <v>0.88049362070908777</v>
+        <v>0.88049362070908765</v>
       </c>
       <c r="V44">
-        <v>0.11950637929091235</v>
+        <v>0.11950637929091233</v>
       </c>
     </row>
     <row r="45">
@@ -1733,16 +1733,16 @@
         <v>67</v>
       </c>
       <c r="B45">
-        <v>0.86237824493402793</v>
+        <v>0.86237824493402782</v>
       </c>
       <c r="C45">
-        <v>0.13762175506597221</v>
+        <v>0.13762175506597216</v>
       </c>
       <c r="H45">
         <v>67</v>
       </c>
       <c r="I45">
-        <v>0.34590733315213584</v>
+        <v>0.34590733315213579</v>
       </c>
       <c r="J45">
         <v>0.65409266684786416</v>
@@ -1771,7 +1771,7 @@
         <v>68</v>
       </c>
       <c r="B46">
-        <v>0.85019651152380527</v>
+        <v>0.85019651152380538</v>
       </c>
       <c r="C46">
         <v>0.14980348847619479</v>
@@ -1783,13 +1783,13 @@
         <v>0.30808878518837662</v>
       </c>
       <c r="J46">
-        <v>0.69191121481162332</v>
+        <v>0.69191121481162343</v>
       </c>
       <c r="N46">
         <v>68</v>
       </c>
       <c r="O46">
-        <v>0.24258895450369605</v>
+        <v>0.24258895450369602</v>
       </c>
       <c r="P46">
         <v>0.757411045496304</v>
@@ -1798,7 +1798,7 @@
         <v>68</v>
       </c>
       <c r="U46">
-        <v>0.87532230895221985</v>
+        <v>0.87532230895221996</v>
       </c>
       <c r="V46">
         <v>0.12467769104778005</v>
@@ -1818,7 +1818,7 @@
         <v>69</v>
       </c>
       <c r="I47">
-        <v>0.3609802330353315</v>
+        <v>0.36098023303533155</v>
       </c>
       <c r="J47">
         <v>0.63901976696466845</v>
@@ -1859,7 +1859,7 @@
         <v>0.33288221829899672</v>
       </c>
       <c r="J48">
-        <v>0.66711778170100322</v>
+        <v>0.66711778170100333</v>
       </c>
       <c r="N48">
         <v>70</v>
@@ -1888,7 +1888,7 @@
         <v>0.84909152218767625</v>
       </c>
       <c r="C49">
-        <v>0.15090847781232375</v>
+        <v>0.15090847781232378</v>
       </c>
       <c r="H49">
         <v>71</v>
@@ -1903,10 +1903,10 @@
         <v>71</v>
       </c>
       <c r="O49">
-        <v>0.32462452159561617</v>
+        <v>0.32462452159561611</v>
       </c>
       <c r="P49">
-        <v>0.67537547840438394</v>
+        <v>0.67537547840438383</v>
       </c>
       <c r="T49">
         <v>71</v>
@@ -1915,7 +1915,7 @@
         <v>0.85819412173868292</v>
       </c>
       <c r="V49">
-        <v>0.14180587826131705</v>
+        <v>0.14180587826131708</v>
       </c>
     </row>
     <row r="50">
@@ -1923,28 +1923,28 @@
         <v>72</v>
       </c>
       <c r="B50">
-        <v>0.82202584326514605</v>
+        <v>0.81926060118652733</v>
       </c>
       <c r="C50">
-        <v>0.17797415673485401</v>
+        <v>0.18073939881347265</v>
       </c>
       <c r="H50">
         <v>72</v>
       </c>
       <c r="I50">
-        <v>0.35371390762291449</v>
+        <v>0.35466569355660404</v>
       </c>
       <c r="J50">
-        <v>0.64628609237708545</v>
+        <v>0.64533430644339596</v>
       </c>
       <c r="N50">
         <v>72</v>
       </c>
       <c r="O50">
-        <v>0.2240481153856474</v>
+        <v>0.22404811538564737</v>
       </c>
       <c r="P50">
-        <v>0.77595188461435272</v>
+        <v>0.7759518846143526</v>
       </c>
       <c r="T50">
         <v>72</v>
@@ -1953,7 +1953,7 @@
         <v>0.84570516614238223</v>
       </c>
       <c r="V50">
-        <v>0.15429483385761777</v>
+        <v>0.1542948338576178</v>
       </c>
     </row>
     <row r="51">
@@ -1961,7 +1961,7 @@
         <v>73</v>
       </c>
       <c r="B51">
-        <v>0.84214408208228497</v>
+        <v>0.84214408208228508</v>
       </c>
       <c r="C51">
         <v>0.15785591791771492</v>
@@ -1970,7 +1970,7 @@
         <v>73</v>
       </c>
       <c r="I51">
-        <v>0.36986695326574676</v>
+        <v>0.3698669532657467</v>
       </c>
       <c r="J51">
         <v>0.6301330467342533</v>
@@ -2002,7 +2002,7 @@
         <v>0.82984200899908267</v>
       </c>
       <c r="C52">
-        <v>0.17015799100091736</v>
+        <v>0.17015799100091733</v>
       </c>
       <c r="H52">
         <v>74</v>
@@ -2011,13 +2011,13 @@
         <v>0.37699773449049984</v>
       </c>
       <c r="J52">
-        <v>0.62300226550950011</v>
+        <v>0.62300226550950022</v>
       </c>
       <c r="N52">
         <v>74</v>
       </c>
       <c r="O52">
-        <v>0.22768528535227739</v>
+        <v>0.22768528535227736</v>
       </c>
       <c r="P52">
         <v>0.77231471464772261</v>
@@ -2037,7 +2037,7 @@
         <v>75</v>
       </c>
       <c r="B53">
-        <v>0.85452926028237308</v>
+        <v>0.85452926028237319</v>
       </c>
       <c r="C53">
         <v>0.14547073971762686</v>
@@ -2055,7 +2055,7 @@
         <v>75</v>
       </c>
       <c r="O53">
-        <v>0.42502006954003352</v>
+        <v>0.42502006954003357</v>
       </c>
       <c r="P53">
         <v>0.57497993045996654</v>
@@ -2064,10 +2064,10 @@
         <v>75</v>
       </c>
       <c r="U53">
-        <v>0.83576238678008974</v>
+        <v>0.83576238678008985</v>
       </c>
       <c r="V53">
-        <v>0.16423761321991023</v>
+        <v>0.16423761321991026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>